<commit_message>
Change made to addresses
</commit_message>
<xml_diff>
--- a/GasPriceScrapper/vendors_address.xlsx
+++ b/GasPriceScrapper/vendors_address.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jake_\Desktop\d3 folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jake_\Documents\GitHub\portfolio\GasPriceScrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6061BDAF-F3E3-4F7C-B109-19FD7BDE2797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791FA670-AB37-4D90-AB05-9F0F9FDA7296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{B0D57C0D-4E6D-4A54-91E9-BDFE107AC331}"/>
   </bookViews>
@@ -84,18 +84,9 @@
     <t>349 Eupeptic Springs Rd, North Carolina</t>
   </si>
   <si>
-    <t>Dad</t>
-  </si>
-  <si>
-    <t>Mamaw</t>
-  </si>
-  <si>
     <t>126 Sharpe Bluff Ln, North Carolina</t>
   </si>
   <si>
-    <t>Kinsley</t>
-  </si>
-  <si>
     <t>121 Pine Valley Dr, Yadkinville, NC 27055</t>
   </si>
   <si>
@@ -133,6 +124,15 @@
   </si>
   <si>
     <t>GE Hitachi Nuclear Energy</t>
+  </si>
+  <si>
+    <t>Eupeptic</t>
+  </si>
+  <si>
+    <t>Cabin</t>
+  </si>
+  <si>
+    <t>Apartments</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -670,10 +670,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>

</xml_diff>